<commit_message>
"Updated 2022 - July "
</commit_message>
<xml_diff>
--- a/src/main/java/config/dataFile.xlsx
+++ b/src/main/java/config/dataFile.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aviraj/git/QA-Automation/src/main/java/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{0BD6C9DE-D153-A44F-BA9D-1F33FBCFFA97}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A147B65E-E9FB-BF4A-A9C9-65ECE7A14F98}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="15800" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>TestCase</t>
   </si>
@@ -43,16 +44,64 @@
     <t>Status</t>
   </si>
   <si>
-    <t>loan</t>
+    <t>Test@123</t>
   </si>
   <si>
-    <t>newsuperadmin2@yopmail.com</t>
+    <t>dummyadmin@yopmail.com</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>companyTrademark</t>
+  </si>
+  <si>
+    <t>companyEmail</t>
+  </si>
+  <si>
+    <t>authorname</t>
+  </si>
+  <si>
+    <t>authoremail</t>
+  </si>
+  <si>
+    <t>adminname</t>
+  </si>
+  <si>
+    <t>adminemail</t>
+  </si>
+  <si>
+    <t>adminlname</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>companyAdmin</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>tester123@yopmail.com</t>
+  </si>
+  <si>
+    <t>qaTesting</t>
+  </si>
+  <si>
+    <t>testingQA</t>
+  </si>
+  <si>
+    <t>admincc11211@yopmail.com</t>
+  </si>
+  <si>
+    <t>testingqates4t1@yopmail.com</t>
   </si>
   <si>
     <t>HC_Company_Creation_01</t>
   </si>
   <si>
-    <t>Test@1234</t>
+    <t>HC_Create_User_2</t>
   </si>
 </sst>
 </file>
@@ -60,7 +109,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +150,19 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF17C694"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -123,7 +185,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="15" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
@@ -133,6 +195,8 @@
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -476,14 +540,18 @@
   <dimension ref="A1:HF3000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" bestFit="true" customWidth="true" style="7" width="26.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" style="3" width="12.1640625" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
@@ -507,21 +575,66 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row ht="19" r="2" spans="1:213" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
       </c>
       <c r="N2" s="2"/>
       <c r="P2" s="6"/>
@@ -545,7 +658,42 @@
       <c r="HE2" s="1"/>
     </row>
     <row ht="19" r="3" spans="1:213" x14ac:dyDescent="0.2">
-      <c r="D3" s="2"/>
+      <c r="A3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
       <c r="N3" s="2"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="5"/>
@@ -12616,7 +12764,28 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2" xr:uid="{07597980-C175-8A4A-81CE-F8383B5EFD77}"/>
+    <hyperlink r:id="rId2" ref="G2" xr:uid="{BF5687FD-935C-8543-84B2-90889A673A81}"/>
+    <hyperlink r:id="rId3" ref="I2" xr:uid="{1A5951A4-4EFE-3E43-AD92-90649098698E}"/>
+    <hyperlink r:id="rId4" ref="K2" xr:uid="{140C4E03-8D96-4443-8DA7-859887055253}"/>
+    <hyperlink r:id="rId5" ref="C3" xr:uid="{23C355AB-EB80-0342-8D3C-3AFCE298A81A}"/>
+    <hyperlink r:id="rId6" ref="G3" xr:uid="{F4730C38-75D7-F743-B4F0-11D8A4CBE05C}"/>
+    <hyperlink r:id="rId7" ref="I3" xr:uid="{3E7CD748-5A81-A54D-AD14-AD262F8F70D1}"/>
+    <hyperlink r:id="rId8" ref="K3" xr:uid="{B3509002-CFBB-664D-AE26-C363C1D04388}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD1BD0C-ADC1-5347-BCFF-FFF8716B01AF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>